<commit_message>
Structuring data and adding it to CSV
</commit_message>
<xml_diff>
--- a/Weather ETL Project Timeline.xlsx
+++ b/Weather ETL Project Timeline.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbubakarDar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Weather ETL Pipeline Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA51818F-D259-4FDC-8132-A4933AD6B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149322DB-CA55-439E-83EE-665A91E79FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C64F887F-764D-4761-AEFC-7EA7859FF7C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tasks</t>
   </si>
@@ -87,6 +76,9 @@
   </si>
   <si>
     <t>More Enhancements</t>
+  </si>
+  <si>
+    <t>Weather Prediction Enhancements</t>
   </si>
 </sst>
 </file>
@@ -448,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963CC950-6842-402F-83AB-8A4848509A4D}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,6 +553,12 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>